<commit_message>
updated pcb for pi2
</commit_message>
<xml_diff>
--- a/razbot_Electronics/razbot_BOM.xlsx
+++ b/razbot_Electronics/razbot_BOM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
   <si>
     <t>Digi PN</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>FUSE BOARD MNT 5A 63VAC/VDC 1206</t>
+  </si>
+  <si>
+    <t>MOTOR CONNECTORS</t>
   </si>
 </sst>
 </file>
@@ -776,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:J35"/>
+  <dimension ref="B4:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1192,7 +1195,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="27.75" customHeight="1">
+    <row r="25" spans="2:10" ht="16.5" customHeight="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
@@ -1440,6 +1443,11 @@
       </c>
       <c r="J35" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>